<commit_message>
Project Plan Configuration for Group is saved. Author: admin. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Plan Configuration for Group/rules/Plan-Configuration-11062015.xlsx
+++ b/DESIGN/rules/Plan Configuration for Group/rules/Plan-Configuration-11062015.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="114">
   <si>
     <t>packageName</t>
   </si>
@@ -848,14 +848,17 @@
   <si>
     <t>FLAT_VALUE_PER_CHILD</t>
   </si>
+  <si>
+    <t>Rules Double[] AvailableMinMaxStepValues ( ReferenceName referenceName, AttributeName attributeName)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="9">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -899,7 +902,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="0" tint="-0.499984740745262"/>
+      <color theme="0" tint="-0.499984740745262" rgb="FFFFFF"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <charset val="204"/>
@@ -926,7 +929,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <charset val="204"/>
@@ -951,7 +954,7 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <charset val="204"/>
@@ -1206,7 +1209,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.59999389629810485" rgb="4F81BD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1218,7 +1221,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1324,7 +1327,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.39997558519241921" rgb="F79646"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2135,268 +2138,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="245">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="9" applyNumberFormat="0" applyProtection="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="4" borderId="10">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="11" applyNumberFormat="0" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" applyNumberFormat="0" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" applyNumberFormat="0" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" applyNumberFormat="0" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="42" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" xfId="3"/>
   </cellStyleXfs>
   <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2456,8 +2202,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="1" xfId="230" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="1" xfId="230" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2501,19 +2247,19 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="24" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2521,10 +2267,10 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="32" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="33" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="32" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="33" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="32" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2536,28 +2282,28 @@
     <xf numFmtId="0" fontId="8" fillId="23" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="37" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="37" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="38" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="38" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="38" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="38" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="41" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="41" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="42" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="42" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="37" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="37" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="41" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="41" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="42" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="42" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2566,49 +2312,49 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="45" xfId="217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="43" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="43" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="39" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="39" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="43" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="43" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="39" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="39" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="35" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="35" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="47" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="47" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="48" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="48" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="36" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="36" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="40" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="40" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="49" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="49" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="50" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="50" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2617,7 +2363,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="50" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="39" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2645,28 +2391,28 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="50" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="50" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="37" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="37" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="55" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="55" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2675,46 +2421,46 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="41" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="41" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="42" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="42" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="59" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="60" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="61" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="53" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="62" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="54" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="51" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="63" xfId="244" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="59" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="60" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="61" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="53" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="62" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="54" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="51" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="63" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2836,10 +2582,10 @@
     <xf numFmtId="0" fontId="12" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="30" fillId="21" borderId="2" xfId="230" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="30" fillId="21" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="30" fillId="21" borderId="4" xfId="230" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="30" fillId="21" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2849,252 +2595,11 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="245">
-    <cellStyle name="20% - Accent1 2" xfId="3"/>
-    <cellStyle name="20% - Accent1 3" xfId="4"/>
-    <cellStyle name="20% - Accent1 4" xfId="5"/>
-    <cellStyle name="20% - Accent1 5" xfId="6"/>
-    <cellStyle name="20% - Accent1 5 2" xfId="7"/>
-    <cellStyle name="20% - Accent1 5 2 2" xfId="8"/>
-    <cellStyle name="20% - Accent1 5 2 2 2" xfId="9"/>
-    <cellStyle name="20% - Accent1 5 2 2_DBASE" xfId="10"/>
-    <cellStyle name="20% - Accent1 5 2 3" xfId="11"/>
-    <cellStyle name="20% - Accent1 5 2_DBASE" xfId="12"/>
-    <cellStyle name="20% - Accent1 5 3" xfId="13"/>
-    <cellStyle name="20% - Accent1 5 3 2" xfId="14"/>
-    <cellStyle name="20% - Accent1 5 3_DBASE" xfId="15"/>
-    <cellStyle name="20% - Accent1 5 4" xfId="16"/>
-    <cellStyle name="20% - Accent1 5_DBASE" xfId="17"/>
-    <cellStyle name="20% - Accent1 6" xfId="18"/>
-    <cellStyle name="20% - Accent1 6 2" xfId="19"/>
-    <cellStyle name="20% - Accent1 6_DBASE" xfId="20"/>
-    <cellStyle name="20% - Accent1 7" xfId="21"/>
-    <cellStyle name="20% - Accent1 8" xfId="22"/>
-    <cellStyle name="20% - Accent2 2" xfId="23"/>
-    <cellStyle name="20% - Accent2 3" xfId="24"/>
-    <cellStyle name="20% - Accent2 4" xfId="25"/>
-    <cellStyle name="20% - Accent3 2" xfId="26"/>
-    <cellStyle name="20% - Accent3 3" xfId="27"/>
-    <cellStyle name="20% - Accent3 4" xfId="28"/>
-    <cellStyle name="20% - Accent4 2" xfId="29"/>
-    <cellStyle name="20% - Accent4 3" xfId="30"/>
-    <cellStyle name="20% - Accent4 4" xfId="31"/>
-    <cellStyle name="20% - Accent5 2" xfId="32"/>
-    <cellStyle name="20% - Accent5 3" xfId="33"/>
-    <cellStyle name="20% - Accent5 4" xfId="34"/>
-    <cellStyle name="20% - Accent6 2" xfId="35"/>
-    <cellStyle name="20% - Accent6 2 2" xfId="36"/>
-    <cellStyle name="20% - Accent6 3" xfId="37"/>
-    <cellStyle name="20% - Accent6 4" xfId="38"/>
-    <cellStyle name="40% - Accent1 2" xfId="39"/>
-    <cellStyle name="40% - Accent1 3" xfId="40"/>
-    <cellStyle name="40% - Accent1 4" xfId="41"/>
-    <cellStyle name="40% - Accent2 2" xfId="42"/>
-    <cellStyle name="40% - Accent2 3" xfId="43"/>
-    <cellStyle name="40% - Accent2 4" xfId="44"/>
-    <cellStyle name="40% - Accent3 2" xfId="45"/>
-    <cellStyle name="40% - Accent3 3" xfId="46"/>
-    <cellStyle name="40% - Accent3 4" xfId="47"/>
-    <cellStyle name="40% - Accent4 2" xfId="48"/>
-    <cellStyle name="40% - Accent4 3" xfId="49"/>
-    <cellStyle name="40% - Accent4 4" xfId="50"/>
-    <cellStyle name="40% - Accent5 2" xfId="51"/>
-    <cellStyle name="40% - Accent5 3" xfId="52"/>
-    <cellStyle name="40% - Accent5 4" xfId="53"/>
-    <cellStyle name="40% - Accent6 2" xfId="54"/>
-    <cellStyle name="40% - Accent6 3" xfId="55"/>
-    <cellStyle name="40% - Accent6 4" xfId="56"/>
-    <cellStyle name="ACT_B" xfId="57"/>
-    <cellStyle name="CD" xfId="58"/>
-    <cellStyle name="Comma 2" xfId="59"/>
-    <cellStyle name="Comma 2 2" xfId="60"/>
-    <cellStyle name="Comma 2 2 2" xfId="61"/>
-    <cellStyle name="Comma 2 2 3" xfId="62"/>
-    <cellStyle name="Comma 2 3" xfId="63"/>
-    <cellStyle name="Comma 2 3 2" xfId="64"/>
-    <cellStyle name="Comma 2 4" xfId="65"/>
-    <cellStyle name="Comma 2 5" xfId="66"/>
-    <cellStyle name="Comma 2 5 2" xfId="67"/>
-    <cellStyle name="Comma 2 6" xfId="68"/>
-    <cellStyle name="Comma 3" xfId="69"/>
-    <cellStyle name="Comma 3 2" xfId="70"/>
-    <cellStyle name="Comma 3 3" xfId="71"/>
-    <cellStyle name="Comma 4" xfId="72"/>
-    <cellStyle name="Comma 5" xfId="73"/>
-    <cellStyle name="Comment" xfId="74"/>
-    <cellStyle name="COND_B" xfId="75"/>
-    <cellStyle name="Currency" xfId="244" builtinId="4"/>
-    <cellStyle name="Currency 2" xfId="76"/>
-    <cellStyle name="Currency 2 2" xfId="77"/>
-    <cellStyle name="Currency 2 2 2" xfId="78"/>
-    <cellStyle name="Currency 2 3" xfId="79"/>
-    <cellStyle name="Currency 2 4" xfId="80"/>
-    <cellStyle name="Currency 2 4 2" xfId="81"/>
-    <cellStyle name="Currency 2 5" xfId="82"/>
-    <cellStyle name="Currency 3" xfId="83"/>
-    <cellStyle name="Currency 3 2" xfId="84"/>
-    <cellStyle name="Currency 3 3" xfId="85"/>
-    <cellStyle name="Currency 4" xfId="86"/>
-    <cellStyle name="Currency 5" xfId="87"/>
-    <cellStyle name="Data type header" xfId="88"/>
-    <cellStyle name="Data type header 2" xfId="89"/>
-    <cellStyle name="Data type header 2 2" xfId="90"/>
-    <cellStyle name="Data type header 2 2 2" xfId="91"/>
-    <cellStyle name="Data type header 2 2 2 2" xfId="92"/>
-    <cellStyle name="Data type header 2 2 3" xfId="93"/>
-    <cellStyle name="Data type header 2 2_DBASE" xfId="94"/>
-    <cellStyle name="Data type header 2 3" xfId="95"/>
-    <cellStyle name="Data type header 2 3 2" xfId="96"/>
-    <cellStyle name="Data type header 2 4" xfId="97"/>
-    <cellStyle name="Data type header 2_DBASE" xfId="98"/>
-    <cellStyle name="Data type header 3" xfId="99"/>
-    <cellStyle name="Data type header 3 2" xfId="100"/>
-    <cellStyle name="Data type header 3 2 2" xfId="101"/>
-    <cellStyle name="Data type header 3 3" xfId="102"/>
-    <cellStyle name="Data type header 3_DBASE" xfId="103"/>
-    <cellStyle name="Data type header 4" xfId="104"/>
-    <cellStyle name="Data type header 4 2" xfId="105"/>
-    <cellStyle name="Data type header 5" xfId="106"/>
-    <cellStyle name="Data type header_DBASE" xfId="107"/>
-    <cellStyle name="Datatype" xfId="108"/>
-    <cellStyle name="Euro" xfId="109"/>
-    <cellStyle name="Euro 2" xfId="110"/>
-    <cellStyle name="H1" xfId="111"/>
-    <cellStyle name="H1 2" xfId="112"/>
-    <cellStyle name="H2" xfId="113"/>
-    <cellStyle name="Heading 1 2" xfId="114"/>
-    <cellStyle name="Heading 2 2" xfId="115"/>
-    <cellStyle name="Hyperlink 2" xfId="116"/>
-    <cellStyle name="Hyperlink 3" xfId="117"/>
-    <cellStyle name="Input 2" xfId="237"/>
-    <cellStyle name="Lien hypertexte 2" xfId="218"/>
-    <cellStyle name="Lien hypertexte 2 2" xfId="219"/>
-    <cellStyle name="Milliers 2" xfId="220"/>
-    <cellStyle name="Milliers 2 2" xfId="221"/>
-    <cellStyle name="Milliers 2 2 2" xfId="222"/>
-    <cellStyle name="Milliers 2 3" xfId="223"/>
-    <cellStyle name="Milliers 3" xfId="224"/>
-    <cellStyle name="Milliers 3 2" xfId="225"/>
-    <cellStyle name="Monétaire 2" xfId="226"/>
-    <cellStyle name="Monétaire 2 2" xfId="227"/>
-    <cellStyle name="Monétaire 3" xfId="228"/>
-    <cellStyle name="Monétaire 3 2" xfId="229"/>
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="118"/>
-    <cellStyle name="Normal 10 2" xfId="119"/>
-    <cellStyle name="Normal 10 2 2" xfId="120"/>
-    <cellStyle name="Normal 10 3" xfId="121"/>
-    <cellStyle name="Normal 10 5" xfId="230"/>
-    <cellStyle name="Normal 10 5 2" xfId="231"/>
-    <cellStyle name="Normal 11" xfId="122"/>
-    <cellStyle name="Normal 11 2" xfId="123"/>
-    <cellStyle name="Normal 11 3" xfId="124"/>
-    <cellStyle name="Normal 12" xfId="125"/>
-    <cellStyle name="Normal 12 2 2 2" xfId="232"/>
-    <cellStyle name="Normal 12 2 2 2 2" xfId="217"/>
-    <cellStyle name="Normal 13" xfId="126"/>
-    <cellStyle name="Normal 13 13 2 2 2 2" xfId="127"/>
-    <cellStyle name="Normal 13 2" xfId="233"/>
-    <cellStyle name="Normal 14" xfId="128"/>
-    <cellStyle name="Normal 15" xfId="129"/>
-    <cellStyle name="Normal 15 2" xfId="130"/>
-    <cellStyle name="Normal 16" xfId="131"/>
-    <cellStyle name="Normal 16 2" xfId="132"/>
-    <cellStyle name="Normal 17" xfId="236"/>
-    <cellStyle name="Normal 2" xfId="133"/>
-    <cellStyle name="Normal 2 2" xfId="1"/>
-    <cellStyle name="Normal 2 2 2" xfId="134"/>
-    <cellStyle name="Normal 2 2 2 2" xfId="135"/>
-    <cellStyle name="Normal 2 2 2 3" xfId="136"/>
-    <cellStyle name="Normal 2 2 2 4" xfId="240"/>
-    <cellStyle name="Normal 2 2 3" xfId="137"/>
-    <cellStyle name="Normal 2 2 4" xfId="138"/>
-    <cellStyle name="Normal 2 2 5" xfId="239"/>
-    <cellStyle name="Normal 2 3" xfId="139"/>
-    <cellStyle name="Normal 2 3 2" xfId="140"/>
-    <cellStyle name="Normal 2 3 2 2" xfId="141"/>
-    <cellStyle name="Normal 2 3 3" xfId="142"/>
-    <cellStyle name="Normal 2 3 4" xfId="143"/>
-    <cellStyle name="Normal 2 3 5" xfId="241"/>
-    <cellStyle name="Normal 2 4" xfId="144"/>
-    <cellStyle name="Normal 2 4 2" xfId="145"/>
-    <cellStyle name="Normal 2 5" xfId="146"/>
-    <cellStyle name="Normal 2 5 2" xfId="147"/>
-    <cellStyle name="Normal 2 5 3" xfId="148"/>
-    <cellStyle name="Normal 2 6" xfId="238"/>
-    <cellStyle name="Normal 3" xfId="2"/>
-    <cellStyle name="Normal 3 2" xfId="149"/>
-    <cellStyle name="Normal 3 2 2" xfId="150"/>
-    <cellStyle name="Normal 3 2 3" xfId="151"/>
-    <cellStyle name="Normal 3 2 4" xfId="242"/>
-    <cellStyle name="Normal 3 3" xfId="152"/>
-    <cellStyle name="Normal 3 3 2" xfId="153"/>
-    <cellStyle name="Normal 3 4" xfId="154"/>
-    <cellStyle name="Normal 3 4 2" xfId="155"/>
-    <cellStyle name="Normal 4" xfId="156"/>
-    <cellStyle name="Normal 4 2" xfId="157"/>
-    <cellStyle name="Normal 4 2 2" xfId="158"/>
-    <cellStyle name="Normal 4 3" xfId="159"/>
-    <cellStyle name="Normal 4 3 2" xfId="160"/>
-    <cellStyle name="Normal 4 3 3" xfId="161"/>
-    <cellStyle name="Normal 4 4" xfId="162"/>
-    <cellStyle name="Normal 5" xfId="163"/>
-    <cellStyle name="Normal 5 2" xfId="164"/>
-    <cellStyle name="Normal 5 2 2" xfId="165"/>
-    <cellStyle name="Normal 5 2 3" xfId="166"/>
-    <cellStyle name="Normal 5 3" xfId="167"/>
-    <cellStyle name="Normal 5 4" xfId="168"/>
-    <cellStyle name="Normal 6" xfId="169"/>
-    <cellStyle name="Normal 6 2" xfId="170"/>
-    <cellStyle name="Normal 6 2 2" xfId="171"/>
-    <cellStyle name="Normal 7" xfId="172"/>
-    <cellStyle name="Normal 7 2" xfId="173"/>
-    <cellStyle name="Normal 7 2 2" xfId="174"/>
-    <cellStyle name="Normal 7 2 3" xfId="175"/>
-    <cellStyle name="Normal 7 3" xfId="176"/>
-    <cellStyle name="Normal 7 3 2" xfId="177"/>
-    <cellStyle name="Normal 7 3 3" xfId="178"/>
-    <cellStyle name="Normal 7 4" xfId="179"/>
-    <cellStyle name="Normal 7 5" xfId="180"/>
-    <cellStyle name="Normal 8" xfId="181"/>
-    <cellStyle name="Normal 8 2" xfId="182"/>
-    <cellStyle name="Normal 8 2 2" xfId="183"/>
-    <cellStyle name="Normal 8 2 3" xfId="184"/>
-    <cellStyle name="Normal 8 3" xfId="185"/>
-    <cellStyle name="Normal 8 3 2" xfId="186"/>
-    <cellStyle name="Normal 9" xfId="187"/>
-    <cellStyle name="Normal 9 2" xfId="188"/>
-    <cellStyle name="Normal 9 2 2" xfId="189"/>
-    <cellStyle name="Normal 9 2 3" xfId="190"/>
-    <cellStyle name="Normal 9 3" xfId="191"/>
-    <cellStyle name="Note 2" xfId="192"/>
-    <cellStyle name="Note 3" xfId="193"/>
-    <cellStyle name="Note 4" xfId="194"/>
-    <cellStyle name="Note 5" xfId="195"/>
-    <cellStyle name="Note 6" xfId="196"/>
-    <cellStyle name="Notification" xfId="197"/>
-    <cellStyle name="Percent 2" xfId="198"/>
-    <cellStyle name="Percent 2 2" xfId="199"/>
-    <cellStyle name="Percent 2 2 2" xfId="200"/>
-    <cellStyle name="Percent 3" xfId="201"/>
-    <cellStyle name="Percent 3 2" xfId="202"/>
-    <cellStyle name="Percent 3 2 2" xfId="203"/>
-    <cellStyle name="Percent 3 3" xfId="204"/>
-    <cellStyle name="Percent 4" xfId="205"/>
-    <cellStyle name="Pourcentage 2" xfId="206"/>
-    <cellStyle name="Pourcentage 2 2" xfId="207"/>
-    <cellStyle name="Pourcentage 2 2 2" xfId="243"/>
-    <cellStyle name="Pourcentage 3" xfId="234"/>
-    <cellStyle name="Pourcentage 3 2" xfId="235"/>
-    <cellStyle name="Гиперссылка 2" xfId="208"/>
-    <cellStyle name="Обычный 2" xfId="209"/>
-    <cellStyle name="Обычный 2 2" xfId="210"/>
-    <cellStyle name="Обычный 3" xfId="211"/>
-    <cellStyle name="Обычный 4" xfId="212"/>
-    <cellStyle name="Обычный 5" xfId="213"/>
-    <cellStyle name="Обычный 5 2" xfId="214"/>
-    <cellStyle name="Обычный 5 3" xfId="215"/>
-    <cellStyle name="Обычный 6" xfId="216"/>
+    <cellStyle name="Normal 12 2 2 2 2" xfId="1"/>
+    <cellStyle name="Normal 10 5" xfId="2"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -4218,9 +3723,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="50.1328125" customWidth="1"/>
-    <col min="5" max="5" width="44" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.73046875" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="50.1328125" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="44.0" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="29.73046875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
@@ -4548,7 +4053,7 @@
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A2:J21"/>
+  <dimension ref="B2:J21"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
@@ -4556,17 +4061,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="21" collapsed="1"/>
-    <col min="2" max="2" width="9.1328125" style="12" collapsed="1"/>
-    <col min="3" max="3" width="43.3984375" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.1328125" style="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.265625" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.59765625" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.73046875" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.59765625" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.1328125" style="12" collapsed="1"/>
-    <col min="10" max="10" width="9.1328125" style="12"/>
-    <col min="11" max="16384" width="9.1328125" style="12" collapsed="1"/>
+    <col min="1" max="1" style="21" width="9.1328125" collapsed="true"/>
+    <col min="2" max="2" style="12" width="9.1328125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="12" width="43.3984375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="22" width="15.1328125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="12" width="20.265625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="12" width="13.59765625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="12" width="14.73046875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="12" width="15.59765625" collapsed="true"/>
+    <col min="9" max="9" style="12" width="9.1328125" collapsed="true"/>
+    <col min="10" max="10" style="12" width="9.1328125" collapsed="false"/>
+    <col min="11" max="16384" style="12" width="9.1328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
@@ -4854,7 +4359,7 @@
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A2:Q15"/>
+  <dimension ref="B2:L15"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
@@ -4862,20 +4367,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="21" collapsed="1"/>
-    <col min="2" max="2" width="9.1328125" style="12" collapsed="1"/>
-    <col min="3" max="3" width="43.3984375" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.86328125" style="12" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.86328125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="16.86328125" style="12" customWidth="1"/>
-    <col min="7" max="8" width="15.86328125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="15.86328125" style="12" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="15.86328125" style="12" customWidth="1"/>
-    <col min="12" max="12" width="9.1328125" style="12" collapsed="1"/>
-    <col min="13" max="15" width="9.1328125" style="12"/>
-    <col min="16" max="16" width="9.1328125" style="12" collapsed="1"/>
-    <col min="17" max="17" width="9.1328125" style="12"/>
-    <col min="18" max="16384" width="9.1328125" style="12" collapsed="1"/>
+    <col min="1" max="1" style="21" width="9.1328125" collapsed="true"/>
+    <col min="2" max="2" style="12" width="9.1328125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="12" width="43.3984375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="12" width="15.86328125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="12" width="15.86328125" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="12" width="16.86328125" collapsed="false"/>
+    <col min="7" max="8" customWidth="true" style="12" width="15.86328125" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="12" width="15.86328125" collapsed="true"/>
+    <col min="10" max="11" customWidth="true" style="12" width="15.86328125" collapsed="false"/>
+    <col min="12" max="12" style="12" width="9.1328125" collapsed="true"/>
+    <col min="13" max="15" style="12" width="9.1328125" collapsed="false"/>
+    <col min="16" max="16" style="12" width="9.1328125" collapsed="true"/>
+    <col min="17" max="17" style="12" width="9.1328125" collapsed="false"/>
+    <col min="18" max="16384" style="12" width="9.1328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="13.15">
@@ -5172,7 +4677,7 @@
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A2:L17"/>
+  <dimension ref="B2:E17"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
@@ -5180,16 +4685,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="21" collapsed="1"/>
-    <col min="2" max="2" width="9.1328125" style="12" collapsed="1"/>
-    <col min="3" max="3" width="58.265625" style="12" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20" style="22" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.1328125" style="12"/>
-    <col min="6" max="6" width="9.1328125" style="12" collapsed="1"/>
-    <col min="7" max="10" width="9.1328125" style="12"/>
-    <col min="11" max="11" width="9.1328125" style="12" collapsed="1"/>
-    <col min="12" max="12" width="9.1328125" style="12"/>
-    <col min="13" max="16384" width="9.1328125" style="12" collapsed="1"/>
+    <col min="1" max="1" style="21" width="9.1328125" collapsed="true"/>
+    <col min="2" max="2" style="12" width="9.1328125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="12" width="58.265625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="22" width="20.0" collapsed="true"/>
+    <col min="5" max="5" style="12" width="9.1328125" collapsed="false"/>
+    <col min="6" max="6" style="12" width="9.1328125" collapsed="true"/>
+    <col min="7" max="10" style="12" width="9.1328125" collapsed="false"/>
+    <col min="11" max="11" style="12" width="9.1328125" collapsed="true"/>
+    <col min="12" max="12" style="12" width="9.1328125" collapsed="false"/>
+    <col min="13" max="16384" style="12" width="9.1328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5">
@@ -5326,7 +4831,7 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A2:P24"/>
+  <dimension ref="B2:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
@@ -5334,17 +4839,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="21" collapsed="1"/>
-    <col min="2" max="2" width="9.1328125" style="12" collapsed="1"/>
-    <col min="3" max="3" width="43.3984375" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.265625" style="22" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.265625" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="8" width="20.265625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="17.265625" style="12" customWidth="1" collapsed="1"/>
-    <col min="10" max="12" width="17.265625" style="12" customWidth="1"/>
-    <col min="13" max="13" width="9.1328125" style="12" collapsed="1"/>
-    <col min="14" max="16" width="9.1328125" style="12"/>
-    <col min="17" max="16384" width="9.1328125" style="12" collapsed="1"/>
+    <col min="1" max="1" style="21" width="9.1328125" collapsed="true"/>
+    <col min="2" max="2" style="12" width="9.1328125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="12" width="43.3984375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="22" width="24.265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="12" width="20.265625" collapsed="true"/>
+    <col min="6" max="8" customWidth="true" style="12" width="20.265625" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="12" width="17.265625" collapsed="true"/>
+    <col min="10" max="12" customWidth="true" style="12" width="17.265625" collapsed="false"/>
+    <col min="13" max="13" style="12" width="9.1328125" collapsed="true"/>
+    <col min="14" max="16" style="12" width="9.1328125" collapsed="false"/>
+    <col min="17" max="16384" style="12" width="9.1328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="13.15">
@@ -5837,7 +5342,7 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A2:O18"/>
+  <dimension ref="B2:L18"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
@@ -5845,20 +5350,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="21" collapsed="1"/>
-    <col min="2" max="2" width="9.1328125" style="12" collapsed="1"/>
-    <col min="3" max="3" width="43.3984375" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.265625" style="22" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.265625" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.265625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="14" style="12" customWidth="1"/>
-    <col min="8" max="8" width="12.73046875" style="12" customWidth="1"/>
-    <col min="9" max="9" width="13" style="12" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.265625" style="12" customWidth="1"/>
-    <col min="11" max="11" width="14.59765625" style="12" customWidth="1"/>
-    <col min="12" max="12" width="9.1328125" style="12" collapsed="1"/>
-    <col min="13" max="15" width="9.1328125" style="12"/>
-    <col min="16" max="16384" width="9.1328125" style="12" collapsed="1"/>
+    <col min="1" max="1" style="21" width="9.1328125" collapsed="true"/>
+    <col min="2" max="2" style="12" width="9.1328125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="12" width="43.3984375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="22" width="24.265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="12" width="20.265625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="12" width="20.265625" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="12" width="14.0" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" style="12" width="12.73046875" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="12" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="12" width="14.265625" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" style="12" width="14.59765625" collapsed="false"/>
+    <col min="12" max="12" style="12" width="9.1328125" collapsed="true"/>
+    <col min="13" max="15" style="12" width="9.1328125" collapsed="false"/>
+    <col min="16" max="16384" style="12" width="9.1328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="13.15">
@@ -6168,7 +5673,7 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A2:AF17"/>
+  <dimension ref="B2:AC17"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
@@ -6176,32 +5681,32 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="21" collapsed="1"/>
-    <col min="2" max="2" width="9.1328125" style="12" collapsed="1"/>
-    <col min="3" max="3" width="43.3984375" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.265625" style="22" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="12.265625" style="22" customWidth="1"/>
-    <col min="7" max="7" width="11.73046875" style="12" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="12.3984375" style="12" customWidth="1"/>
-    <col min="10" max="10" width="9.3984375" style="12" customWidth="1"/>
-    <col min="11" max="11" width="6.59765625" style="12" customWidth="1"/>
-    <col min="12" max="12" width="6.265625" style="12" customWidth="1"/>
-    <col min="13" max="13" width="6.73046875" style="12" customWidth="1"/>
-    <col min="14" max="15" width="6.265625" style="12" customWidth="1"/>
-    <col min="16" max="16" width="6.1328125" style="12" customWidth="1"/>
-    <col min="17" max="18" width="11.73046875" style="12" customWidth="1"/>
-    <col min="19" max="19" width="11" style="12" customWidth="1" collapsed="1"/>
-    <col min="20" max="21" width="10.59765625" style="12" customWidth="1"/>
-    <col min="22" max="22" width="12.3984375" style="12" customWidth="1"/>
-    <col min="23" max="23" width="6.59765625" style="12" customWidth="1"/>
-    <col min="24" max="24" width="6.86328125" style="12" customWidth="1"/>
-    <col min="25" max="25" width="5.86328125" style="12" customWidth="1"/>
-    <col min="26" max="26" width="6.1328125" style="12" customWidth="1"/>
-    <col min="27" max="27" width="5.86328125" style="12" customWidth="1"/>
-    <col min="28" max="28" width="6.59765625" style="12" customWidth="1"/>
-    <col min="29" max="29" width="9.1328125" style="12" collapsed="1"/>
-    <col min="30" max="32" width="9.1328125" style="12"/>
-    <col min="33" max="16384" width="9.1328125" style="12" collapsed="1"/>
+    <col min="1" max="1" style="21" width="9.1328125" collapsed="true"/>
+    <col min="2" max="2" style="12" width="9.1328125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="12" width="43.3984375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="22" width="24.265625" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" style="22" width="12.265625" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="12" width="11.73046875" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" style="12" width="12.3984375" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" style="12" width="9.3984375" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" style="12" width="6.59765625" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" style="12" width="6.265625" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" style="12" width="6.73046875" collapsed="false"/>
+    <col min="14" max="15" customWidth="true" style="12" width="6.265625" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" style="12" width="6.1328125" collapsed="false"/>
+    <col min="17" max="18" customWidth="true" style="12" width="11.73046875" collapsed="false"/>
+    <col min="19" max="19" customWidth="true" style="12" width="11.0" collapsed="true"/>
+    <col min="20" max="21" customWidth="true" style="12" width="10.59765625" collapsed="false"/>
+    <col min="22" max="22" customWidth="true" style="12" width="12.3984375" collapsed="false"/>
+    <col min="23" max="23" customWidth="true" style="12" width="6.59765625" collapsed="false"/>
+    <col min="24" max="24" customWidth="true" style="12" width="6.86328125" collapsed="false"/>
+    <col min="25" max="25" customWidth="true" style="12" width="5.86328125" collapsed="false"/>
+    <col min="26" max="26" customWidth="true" style="12" width="6.1328125" collapsed="false"/>
+    <col min="27" max="27" customWidth="true" style="12" width="5.86328125" collapsed="false"/>
+    <col min="28" max="28" customWidth="true" style="12" width="6.59765625" collapsed="false"/>
+    <col min="29" max="29" style="12" width="9.1328125" collapsed="true"/>
+    <col min="30" max="32" style="12" width="9.1328125" collapsed="false"/>
+    <col min="33" max="16384" style="12" width="9.1328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="13.15">
@@ -6327,7 +5832,7 @@
     <row r="6" spans="2:29" ht="15.75" customHeight="1" thickBot="1">
       <c r="B6" s="10"/>
       <c r="C6" s="140" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="D6" s="141"/>
       <c r="E6" s="141"/>
@@ -6819,10 +6324,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="9.1328125" style="12" collapsed="1"/>
-    <col min="3" max="3" width="16.86328125" style="12" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="34.265625" style="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.1328125" style="12" collapsed="1"/>
+    <col min="1" max="2" style="12" width="9.1328125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="12" width="16.86328125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="12" width="34.265625" collapsed="true"/>
+    <col min="5" max="16384" style="12" width="9.1328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5">

</xml_diff>